<commit_message>
added support for names collection with xw server
</commit_message>
<xml_diff>
--- a/tests/test_engines/engines.xlsx
+++ b/tests/test_engines/engines.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/test_json/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/test_engines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32902394-7514-6545-A425-3CBF8F9E41E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA6C9F2-D31E-DC46-A4F8-630EBD0B4223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3960" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{122BE06B-C62B-364D-8C27-94A5A3A52BCE}"/>
   </bookViews>
@@ -120,6 +120,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="mypic1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8C6308A-77C6-9700-C479-E17461BAD874}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5753100" y="1866900"/>
+          <a:ext cx="254000" cy="127000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="mypic2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{016C4711-D9BC-0D58-C00A-8F6A2533F52A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4902200" y="4343400"/>
+          <a:ext cx="508000" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -422,7 +515,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -472,6 +567,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
more tests and fixes
</commit_message>
<xml_diff>
--- a/tests/test_engines/engines.xlsx
+++ b/tests/test_engines/engines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/test_engines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC74675-FF71-AF47-B52C-C147F067F721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B50457-92A3-ED40-858B-F444C8588C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3960" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{122BE06B-C62B-364D-8C27-94A5A3A52BCE}"/>
   </bookViews>
@@ -69,7 +69,7 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Bye xlwings!</t>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -565,6 +565,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_XLWINGS_ADD</we:customFunctionIds>
@@ -581,7 +584,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>